<commit_message>
Changes included to scripts
</commit_message>
<xml_diff>
--- a/Test Data/Navigation/Navigation.xlsx
+++ b/Test Data/Navigation/Navigation.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cloud01" sheetId="1" r:id="rId1"/>
+    <sheet name="Cloud02" sheetId="2" r:id="rId2"/>
+    <sheet name="Cloud03" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="67">
   <si>
     <t>Screen</t>
   </si>
@@ -302,6 +304,48 @@
   </si>
   <si>
     <t>Invoice Print</t>
+  </si>
+  <si>
+    <t>Transactions;Receivables;Invoice;Sales Invoice</t>
+  </si>
+  <si>
+    <t>Upload Utility;Sales Order Upload</t>
+  </si>
+  <si>
+    <t>Transactions;Receivables;Orders;Order History</t>
+  </si>
+  <si>
+    <t>Transactions;Receivables;Orders;Stock Allocation [Queue]</t>
+  </si>
+  <si>
+    <t>Transactions;Receivables;Orders;View Allocation [Queue]</t>
+  </si>
+  <si>
+    <t>Transactions;Receivables;Orders;Swap SuBF</t>
+  </si>
+  <si>
+    <t>Transactions;Receivables;Returns;SRN - With Reference</t>
+  </si>
+  <si>
+    <t>Sales Invoice</t>
+  </si>
+  <si>
+    <t>Sales Order Upload</t>
+  </si>
+  <si>
+    <t>Order History</t>
+  </si>
+  <si>
+    <t>Swap SuBF</t>
+  </si>
+  <si>
+    <t>SRN - With Reference</t>
+  </si>
+  <si>
+    <t>Stock Allocation</t>
+  </si>
+  <si>
+    <t>View Allocation</t>
   </si>
 </sst>
 </file>
@@ -813,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D28"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1366,6 +1410,118 @@
         <v>2</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1374,4 +1530,1348 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.6328125" style="1" customWidth="1"/>
+    <col min="1013" max="1024" width="11.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="11">
+        <v>7</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="11">
+        <v>8</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="11">
+        <v>9</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="11">
+        <v>11</v>
+      </c>
+      <c r="D12" s="11">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11">
+        <v>12</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="12">
+        <v>13</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="12">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12">
+        <v>15</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.6328125" style="1" customWidth="1"/>
+    <col min="1013" max="1024" width="11.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="11">
+        <v>7</v>
+      </c>
+      <c r="D8" s="11">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="11">
+        <v>8</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="11">
+        <v>9</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="11">
+        <v>11</v>
+      </c>
+      <c r="D12" s="11">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11">
+        <v>12</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="12">
+        <v>13</v>
+      </c>
+      <c r="D14" s="12">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="12">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" ht="13" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12">
+        <v>15</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>